<commit_message>
update default inf temp
</commit_message>
<xml_diff>
--- a/exposan/metab/data/analysis_framework.xlsx
+++ b/exposan/metab/data/analysis_framework.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joy_c\Dropbox\PhD\Research\METAB-DOE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joy_c\Dropbox\PhD\Research\QSD\codes_developing\EXPOsan\exposan\metab\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{658BCF72-FB29-4574-9CB7-E9FC6A2CEF38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{131DF3B0-8A79-47BA-B0B7-5B507A01298C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-75" windowWidth="29040" windowHeight="15720" activeTab="9" xr2:uid="{E43D8F4A-1C25-4B70-B048-7C6086C991E6}"/>
+    <workbookView xWindow="-25320" yWindow="1860" windowWidth="21510" windowHeight="12900" firstSheet="2" activeTab="10" xr2:uid="{E43D8F4A-1C25-4B70-B048-7C6086C991E6}"/>
   </bookViews>
   <sheets>
     <sheet name="DV" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="103">
   <si>
     <t># of stages</t>
   </si>
@@ -1007,7 +1007,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1037,13 +1037,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1065,13 +1058,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2006,7 +1998,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80E9A887-5507-4CA1-91AE-8B8ED7331C2F}">
   <dimension ref="A1:F145"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
@@ -5069,8 +5061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18B9082E-E44E-4B83-A023-B5F2F184D914}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5263,6 +5255,9 @@
       <c r="G8" t="s">
         <v>94</v>
       </c>
+      <c r="H8" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
@@ -5278,6 +5273,9 @@
       <c r="G9" t="s">
         <v>94</v>
       </c>
+      <c r="H9" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
@@ -5293,7 +5291,9 @@
       <c r="G10" t="s">
         <v>94</v>
       </c>
-      <c r="H10" s="3"/>
+      <c r="H10" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">

</xml_diff>

<commit_message>
add functions to breakdown impacts
</commit_message>
<xml_diff>
--- a/exposan/metab/data/analysis_framework.xlsx
+++ b/exposan/metab/data/analysis_framework.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joy_c\Dropbox\PhD\Research\QSD\codes_developing\EXPOsan\exposan\metab\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{131DF3B0-8A79-47BA-B0B7-5B507A01298C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{654FD2BA-EF1E-4CF6-A09E-E1451B56BAFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="1860" windowWidth="21510" windowHeight="12900" firstSheet="2" activeTab="10" xr2:uid="{E43D8F4A-1C25-4B70-B048-7C6086C991E6}"/>
+    <workbookView xWindow="-22980" yWindow="525" windowWidth="20670" windowHeight="12345" firstSheet="2" activeTab="10" xr2:uid="{E43D8F4A-1C25-4B70-B048-7C6086C991E6}"/>
   </bookViews>
   <sheets>
     <sheet name="DV" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="118">
   <si>
     <t># of stages</t>
   </si>
@@ -943,9 +943,6 @@
     <t># combo</t>
   </si>
   <si>
-    <t>(1000, 1860)</t>
-  </si>
-  <si>
     <t>Temperature</t>
   </si>
   <si>
@@ -1002,6 +999,54 @@
   <si>
     <t>Bead diameter</t>
   </si>
+  <si>
+    <t>FluidizedBed</t>
+  </si>
+  <si>
+    <t>FB voidage</t>
+  </si>
+  <si>
+    <t>(0.6, 0.9)</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>(1, 5)</t>
+  </si>
+  <si>
+    <t>(effluent only)</t>
+  </si>
+  <si>
+    <t>HRT</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>(1/6, 2)</t>
+  </si>
+  <si>
+    <t>(990, 1860)</t>
+  </si>
+  <si>
+    <t>height-to-diameter ratio</t>
+  </si>
+  <si>
+    <t>(1, 4)</t>
+  </si>
+  <si>
+    <t>(0.5, 2)</t>
+  </si>
+  <si>
+    <t>Bead lifetime</t>
+  </si>
+  <si>
+    <t>yr</t>
+  </si>
+  <si>
+    <t>(1, 10)</t>
+  </si>
 </sst>
 </file>
 
@@ -1038,12 +1083,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1058,12 +1109,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1398,7 +1451,7 @@
   <sheetData>
     <row r="1" spans="1:22" s="1" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1413,7 +1466,7 @@
         <v>20</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>21</v>
@@ -1437,7 +1490,7 @@
         <v>15</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>13</v>
@@ -1458,7 +1511,7 @@
         <v>8</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
@@ -1503,7 +1556,7 @@
         <v>12</v>
       </c>
       <c r="O2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P2">
         <v>2</v>
@@ -1524,7 +1577,7 @@
         <v>6</v>
       </c>
       <c r="V2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
@@ -1569,7 +1622,7 @@
         <v>4</v>
       </c>
       <c r="O3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P3">
         <v>5</v>
@@ -1590,7 +1643,7 @@
         <v>7</v>
       </c>
       <c r="V3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
@@ -2010,10 +2063,10 @@
   <sheetData>
     <row r="1" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>19</v>
@@ -2022,10 +2075,10 @@
         <v>81</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -5059,10 +5112,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18B9082E-E44E-4B83-A023-B5F2F184D914}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5094,360 +5147,487 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2">
-        <v>0.39</v>
-      </c>
-      <c r="E2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" t="s">
-        <v>76</v>
-      </c>
-      <c r="H2" t="s">
-        <v>77</v>
-      </c>
-      <c r="I2" t="s">
-        <v>78</v>
-      </c>
+    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D3">
-        <v>16</v>
+        <v>0.39</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G3" t="s">
-        <v>40</v>
+        <v>76</v>
+      </c>
+      <c r="H3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I3" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>112</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D4">
-        <v>1420</v>
+        <v>1.5</v>
       </c>
       <c r="E4" t="s">
-        <v>47</v>
+        <v>91</v>
       </c>
       <c r="F4" t="s">
-        <v>83</v>
-      </c>
-      <c r="G4" t="s">
-        <v>40</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="G4" s="4"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>102</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>103</v>
       </c>
       <c r="C5" t="s">
         <v>25</v>
       </c>
       <c r="D5">
-        <v>0.55000000000000004</v>
+        <v>0.75</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>91</v>
       </c>
       <c r="F5" t="s">
-        <v>38</v>
-      </c>
-      <c r="G5" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5" t="s">
-        <v>39</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>102</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>112</v>
       </c>
       <c r="C6" t="s">
         <v>25</v>
       </c>
       <c r="D6">
-        <v>0.96299999999999997</v>
+        <v>1.5</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>91</v>
       </c>
       <c r="F6" t="s">
-        <v>79</v>
-      </c>
-      <c r="G6" t="s">
-        <v>48</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7">
+        <v>16</v>
+      </c>
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8">
+        <v>1420</v>
+      </c>
+      <c r="E8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" t="s">
+        <v>111</v>
+      </c>
+      <c r="G8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>91</v>
+      </c>
+      <c r="F10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C11" t="s">
+        <v>116</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
+        <v>91</v>
+      </c>
+      <c r="F11" t="s">
+        <v>117</v>
+      </c>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12">
+        <v>0.96299999999999997</v>
+      </c>
+      <c r="E12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" t="s">
+        <v>79</v>
+      </c>
+      <c r="G12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>51</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B13" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13">
+        <v>0.5</v>
+      </c>
+      <c r="E13" t="s">
         <v>91</v>
       </c>
-      <c r="C7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7">
-        <v>0.5</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="F13" t="s">
         <v>92</v>
       </c>
-      <c r="F7" t="s">
-        <v>93</v>
-      </c>
-      <c r="G7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="G13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>107</v>
+      </c>
+      <c r="B14" t="s">
         <v>41</v>
       </c>
-      <c r="D8">
+      <c r="D14">
         <f>(0.55+0.7)/2</f>
         <v>0.625</v>
       </c>
-      <c r="F8" t="s">
-        <v>97</v>
-      </c>
-      <c r="G8" t="s">
-        <v>94</v>
-      </c>
-      <c r="H8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="F14" t="s">
+        <v>96</v>
+      </c>
+      <c r="G14" t="s">
+        <v>93</v>
+      </c>
+      <c r="H14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>42</v>
       </c>
-      <c r="D9">
+      <c r="D15">
         <f>(0.36 + 0.55)/2</f>
         <v>0.45500000000000002</v>
       </c>
-      <c r="F9" t="s">
-        <v>96</v>
-      </c>
-      <c r="G9" t="s">
-        <v>94</v>
-      </c>
-      <c r="H9" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="F15" t="s">
+        <v>95</v>
+      </c>
+      <c r="G15" t="s">
+        <v>93</v>
+      </c>
+      <c r="H15" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>43</v>
       </c>
-      <c r="D10">
+      <c r="D16">
         <f>(0.06+0.2)/2</f>
         <v>0.13</v>
       </c>
-      <c r="F10" t="s">
-        <v>95</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="F16" t="s">
         <v>94</v>
       </c>
-      <c r="H10" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="G16" t="s">
+        <v>93</v>
+      </c>
+      <c r="H16" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>53</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B17" t="s">
         <v>54</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C17" t="s">
         <v>61</v>
       </c>
-      <c r="D11">
+      <c r="D17">
         <v>8</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E17" t="s">
         <v>23</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F17" t="s">
         <v>63</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G17" t="s">
         <v>69</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H17" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>53</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B18" t="s">
         <v>55</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C18" t="s">
         <v>62</v>
       </c>
-      <c r="D12">
+      <c r="D18">
         <v>0.15</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E18" t="s">
         <v>23</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F18" t="s">
         <v>64</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G18" t="s">
         <v>70</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H18" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>53</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B19" t="s">
         <v>56</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C19" t="s">
         <v>61</v>
       </c>
-      <c r="D13">
+      <c r="D19">
         <v>13</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E19" t="s">
         <v>23</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F19" t="s">
         <v>65</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G19" t="s">
         <v>71</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H19" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>53</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B20" t="s">
         <v>57</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C20" t="s">
         <v>62</v>
       </c>
-      <c r="D14">
+      <c r="D20">
         <v>0.1</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E20" t="s">
         <v>23</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F20" t="s">
         <v>66</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G20" t="s">
         <v>72</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H20" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>53</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B21" t="s">
         <v>58</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C21" t="s">
         <v>61</v>
       </c>
-      <c r="D15">
+      <c r="D21">
         <v>6</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E21" t="s">
         <v>23</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F21" t="s">
         <v>67</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G21" t="s">
         <v>73</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H21" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>53</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B22" t="s">
         <v>59</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C22" t="s">
         <v>60</v>
       </c>
-      <c r="D16">
+      <c r="D22">
         <v>0.02</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E22" t="s">
         <v>23</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F22" t="s">
         <v>68</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G22" t="s">
         <v>74</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H22" t="s">
         <v>75</v>
       </c>
     </row>
@@ -5473,13 +5653,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -5590,16 +5770,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5958,19 +6138,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -7218,16 +7398,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -7475,19 +7655,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -8327,22 +8507,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -11246,16 +11426,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>81</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -11519,19 +11699,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>81</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>